<commit_message>
update ul excel manager
update ul excel manager
handle fe translations
</commit_message>
<xml_diff>
--- a/FILE_MANAGER/App_Data/UL/sample_source/lookups_translations.xlsx
+++ b/FILE_MANAGER/App_Data/UL/sample_source/lookups_translations.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\107758\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\107758\Documents\GitHubMaster\FileManagerTool\FILE_MANAGER\App_Data\UL\sample_source\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D248EA34-E11B-456A-BDC1-513CDC4BBFD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA8A28DE-C2DA-46E4-BC9A-3D883159CF88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="313" activeTab="1" xr2:uid="{3310C5B7-088C-4A23-ACEB-6DE97B5B93CB}"/>
   </bookViews>
@@ -2315,7 +2315,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E19" sqref="E19"/>
+      <selection pane="bottomRight" activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>